<commit_message>
refresh : (salah pull kemarin)
</commit_message>
<xml_diff>
--- a/public/templates/template_siswa.xlsx
+++ b/public/templates/template_siswa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\akademik\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FDCBEA-2514-41FF-B40D-F0DF91111EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C62624-851A-499F-8ED0-D04D1C32ACBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3192" yWindow="348" windowWidth="17280" windowHeight="9420" xr2:uid="{208537F3-6AD5-4600-AF24-3E175ED132CB}"/>
+    <workbookView xWindow="3540" yWindow="696" windowWidth="17280" windowHeight="9420" xr2:uid="{208537F3-6AD5-4600-AF24-3E175ED132CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>NIS</t>
-  </si>
-  <si>
     <t>NAMA</t>
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>NISN</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,13 +421,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>